<commit_message>
update recentContact to  recentChat
</commit_message>
<xml_diff>
--- a/doc/db/aiTalkDB_Backend.xlsx
+++ b/doc/db/aiTalkDB_Backend.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chenqingze/Workspace/Repositories/aitalk/doc/db/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02CB7A6C-A354-484D-9DAF-8A0C88B1599A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE552F6F-D452-7040-813C-2C6CC0142C6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="772" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="772" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="修订历史" sheetId="12" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <sheet name="notification" sheetId="7" r:id="rId11"/>
     <sheet name="tmpConversation" sheetId="20" r:id="rId12"/>
     <sheet name="resource" sheetId="10" r:id="rId13"/>
-    <sheet name="recentContact" sheetId="21" r:id="rId14"/>
+    <sheet name="recentChat" sheetId="21" r:id="rId14"/>
     <sheet name="店铺咨询逻辑" sheetId="25" r:id="rId15"/>
   </sheets>
   <calcPr calcId="144525"/>
@@ -745,12 +745,6 @@
     <t>消息类型0：文本 1：音频 2：视频 3：位置 4：名片 5：图片 6：讯息 7：团购 8：通知 9：商品 10：易货 11：店铺  12： 抢单 13：群聊邀请 14:群通知 15 文件 16 通知 17回复 18 @  19 预购单 20 配送 21 动态</t>
   </si>
   <si>
-    <t>recentContact</t>
-  </si>
-  <si>
-    <t>最近联系人</t>
-  </si>
-  <si>
     <t>点对点通信历史消息（点对点消息归档）</t>
   </si>
   <si>
@@ -941,6 +935,12 @@
   </si>
   <si>
     <t>关注/订阅/粉丝关系</t>
+  </si>
+  <si>
+    <t>recentChat</t>
+  </si>
+  <si>
+    <t>最近消息/最近联系人</t>
   </si>
 </sst>
 </file>
@@ -3918,7 +3918,7 @@
         <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -3945,7 +3945,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B6" t="s">
         <v>25</v>
@@ -4042,11 +4042,11 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="53" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B3" s="53"/>
       <c r="C3" s="53" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -4055,16 +4055,16 @@
       </c>
       <c r="B4" s="49"/>
       <c r="C4" s="49" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="49" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B5" s="49"/>
       <c r="C5" s="49" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -4073,16 +4073,16 @@
       </c>
       <c r="B6" s="49"/>
       <c r="C6" s="49" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="49" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B7" s="49"/>
       <c r="C7" s="49" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -4091,7 +4091,7 @@
       </c>
       <c r="B8" s="49"/>
       <c r="C8" s="49" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -4100,7 +4100,7 @@
       </c>
       <c r="B9" s="49"/>
       <c r="C9" s="49" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -4118,7 +4118,7 @@
       </c>
       <c r="B11" s="49"/>
       <c r="C11" s="49" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -4127,7 +4127,7 @@
       </c>
       <c r="B12" s="49"/>
       <c r="C12" s="49" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -4358,7 +4358,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4399,18 +4399,18 @@
         <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -4437,13 +4437,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B7" t="s">
         <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -4459,7 +4459,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B9" t="s">
         <v>25</v>
@@ -4547,13 +4547,13 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B17" t="s">
         <v>18</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -4897,8 +4897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -4931,7 +4931,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="47" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B3" s="23" t="s">
         <v>111</v>
@@ -4940,7 +4940,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="47" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B4" s="40" t="s">
         <v>101</v>
@@ -4960,10 +4960,10 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="55" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B6" s="56" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C6" s="41"/>
     </row>
@@ -4972,7 +4972,7 @@
         <v>109</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C7" s="19" t="s">
         <v>115</v>
@@ -4980,7 +4980,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="47" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>102</v>
@@ -5002,7 +5002,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="47" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B10" s="35" t="s">
         <v>135</v>
@@ -5011,7 +5011,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="51" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B11" s="18" t="s">
         <v>100</v>
@@ -5048,19 +5048,19 @@
       <c r="C14" s="33"/>
     </row>
     <row r="15" spans="1:4" s="5" customFormat="1">
-      <c r="A15" s="21" t="s">
-        <v>170</v>
-      </c>
-      <c r="B15" s="21" t="s">
-        <v>171</v>
-      </c>
-      <c r="C15" s="21" t="s">
-        <v>201</v>
+      <c r="A15" s="23" t="s">
+        <v>234</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>235</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="25" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B16" s="22" t="s">
         <v>144</v>
@@ -5082,18 +5082,18 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="24" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B18" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="C18" s="21" t="s">
         <v>174</v>
-      </c>
-      <c r="C18" s="21" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="25" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B19" s="22" t="s">
         <v>107</v>
@@ -5102,7 +5102,7 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="24" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B20" s="21" t="s">
         <v>112</v>
@@ -5124,7 +5124,7 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="52" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -5201,27 +5201,27 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="46" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B5" s="46" t="s">
         <v>25</v>
       </c>
       <c r="C5" s="46" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -5229,18 +5229,18 @@
         <v>20</v>
       </c>
       <c r="B7" s="46" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C7" t="s">
         <v>21</v>
       </c>
       <c r="D7" s="46" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="C8" s="46" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D8" s="46"/>
     </row>
@@ -5252,33 +5252,33 @@
     </row>
     <row r="10" spans="1:4">
       <c r="C10" s="46" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D10" s="46"/>
     </row>
     <row r="11" spans="1:4">
       <c r="C11" s="46" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D11" s="46"/>
     </row>
     <row r="12" spans="1:4">
       <c r="B12" s="46"/>
       <c r="C12" s="46" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D12" s="46"/>
     </row>
     <row r="13" spans="1:4">
       <c r="B13" s="46"/>
       <c r="C13" s="46" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D13" s="46"/>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="30" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B14" t="s">
         <v>22</v>
@@ -5427,7 +5427,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="53" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B7" t="s">
         <v>25</v>
@@ -5436,7 +5436,7 @@
         <v>33</v>
       </c>
       <c r="D7" s="57" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E7" s="3"/>
     </row>
@@ -5478,7 +5478,7 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B11" s="30" t="s">
         <v>25</v>
@@ -5596,35 +5596,35 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="46" t="s">
+        <v>191</v>
+      </c>
+      <c r="B6" s="46" t="s">
+        <v>190</v>
+      </c>
+      <c r="C6" s="46" t="s">
         <v>193</v>
-      </c>
-      <c r="B6" s="46" t="s">
-        <v>192</v>
-      </c>
-      <c r="C6" s="46" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="46" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B7" s="50" t="s">
+        <v>190</v>
+      </c>
+      <c r="C7" s="46" t="s">
         <v>192</v>
-      </c>
-      <c r="C7" s="46" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="49" customFormat="1">
       <c r="A8" s="49" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B8" s="49" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C8" s="49" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -5717,7 +5717,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="53" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B5" t="s">
         <v>25</v>
@@ -5728,7 +5728,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="53" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B6" t="s">
         <v>22</v>
@@ -5737,7 +5737,7 @@
         <v>123</v>
       </c>
       <c r="D6" s="53" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -5756,7 +5756,7 @@
         <v>117</v>
       </c>
       <c r="B8" s="48" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C8" t="s">
         <v>125</v>
@@ -5861,7 +5861,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -5906,7 +5906,7 @@
         <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -5917,7 +5917,7 @@
         <v>16</v>
       </c>
       <c r="C4" s="53" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -5928,7 +5928,7 @@
         <v>16</v>
       </c>
       <c r="C5" s="53" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -5944,13 +5944,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B7" t="s">
         <v>25</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -6006,7 +6006,7 @@
         <v>25</v>
       </c>
       <c r="C12" s="38" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="69" spans="3:3">
@@ -6068,7 +6068,7 @@
         <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -6106,7 +6106,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B7" t="s">
         <v>25</v>

</xml_diff>